<commit_message>
Atualizados mapas do IQ_DOC*
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IQ_DOC.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IQ_DOC.XLSX
@@ -130,7 +130,7 @@
     <t>Domingo</t>
   </si>
   <si>
-    <t>ROBERTO O.SHINAGAWA</t>
+    <t>JOAO CARLOS DE OLIVEIRA CRUZ</t>
   </si>
   <si>
     <t>LUIZ FERNANDO LIMA DIAS</t>
@@ -148,7 +148,7 @@
     <t> </t>
   </si>
   <si>
-    <t>528</t>
+    <t>2899</t>
   </si>
   <si>
     <t>3219</t>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="M12" s="174" t="str">
         <f>G12</f>
-        <v>ROBERTO O.SHINAGAWA</v>
+        <v>JOAO CARLOS DE OLIVEIRA CRUZ</v>
       </c>
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
@@ -3545,7 +3545,7 @@
       <c r="T12" s="189"/>
       <c r="U12" s="174" t="str">
         <f>G12</f>
-        <v>ROBERTO O.SHINAGAWA</v>
+        <v>JOAO CARLOS DE OLIVEIRA CRUZ</v>
       </c>
       <c r="V12" s="161"/>
       <c r="W12" s="161"/>
@@ -3571,7 +3571,7 @@
       </c>
       <c r="AC12" s="181" t="str">
         <f t="shared" ref="AC12:AH12" si="0">G12</f>
-        <v>ROBERTO O.SHINAGAWA</v>
+        <v>JOAO CARLOS DE OLIVEIRA CRUZ</v>
       </c>
       <c r="AD12" s="183" t="str">
         <f t="shared" si="0"/>
@@ -3595,7 +3595,7 @@
       </c>
       <c r="AI12" s="185" t="str">
         <f t="shared" ref="AI12:AN12" si="1">G12</f>
-        <v>ROBERTO O.SHINAGAWA</v>
+        <v>JOAO CARLOS DE OLIVEIRA CRUZ</v>
       </c>
       <c r="AJ12" s="183" t="str">
         <f t="shared" si="1"/>
@@ -3899,7 +3899,7 @@
       </c>
       <c r="M19" s="191" t="str">
         <f>G19</f>
-        <v>528</v>
+        <v>2899</v>
       </c>
       <c r="N19" s="172"/>
       <c r="O19" s="172" t="str">
@@ -3925,7 +3925,7 @@
       <c r="T19" s="209"/>
       <c r="U19" s="191" t="str">
         <f>G19</f>
-        <v>528</v>
+        <v>2899</v>
       </c>
       <c r="V19" s="172"/>
       <c r="W19" s="172"/>
@@ -3951,7 +3951,7 @@
       </c>
       <c r="AC19" s="207" t="str">
         <f t="shared" ref="AC19:AH19" si="2">G19</f>
-        <v>528</v>
+        <v>2899</v>
       </c>
       <c r="AD19" s="172" t="str">
         <f t="shared" si="2"/>
@@ -3975,7 +3975,7 @@
       </c>
       <c r="AI19" s="205" t="str">
         <f t="shared" ref="AI19:AN19" si="3">G19</f>
-        <v>528</v>
+        <v>2899</v>
       </c>
       <c r="AJ19" s="172" t="str">
         <f t="shared" si="3"/>
@@ -6605,7 +6605,7 @@
       <c r="F12" s="159"/>
       <c r="G12" s="174" t="str">
         <f>'Segunda a Sexta'!G12:G18</f>
-        <v>ROBERTO O.SHINAGAWA</v>
+        <v>JOAO CARLOS DE OLIVEIRA CRUZ</v>
       </c>
       <c r="H12" s="161" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
@@ -6629,7 +6629,7 @@
       </c>
       <c r="M12" s="174" t="str">
         <f>'Segunda a Sexta'!G12:G18</f>
-        <v>ROBERTO O.SHINAGAWA</v>
+        <v>JOAO CARLOS DE OLIVEIRA CRUZ</v>
       </c>
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
@@ -6937,7 +6937,7 @@
       </c>
       <c r="G19" s="258" t="str">
         <f>'Segunda a Sexta'!G19:G20</f>
-        <v>528</v>
+        <v>2899</v>
       </c>
       <c r="H19" s="168" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
@@ -6961,7 +6961,7 @@
       </c>
       <c r="M19" s="191" t="str">
         <f>'Segunda a Sexta'!G19:G20</f>
-        <v>528</v>
+        <v>2899</v>
       </c>
       <c r="N19" s="172"/>
       <c r="O19" s="257" t="str">

</xml_diff>